<commit_message>
species id's are finished.  ready for plotting
</commit_message>
<xml_diff>
--- a/raw_data/species_list.xlsx
+++ b/raw_data/species_list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="77">
   <si>
     <t>Angiosperm</t>
   </si>
@@ -581,6 +581,75 @@
   </si>
   <si>
     <t>vio_sp</t>
+  </si>
+  <si>
+    <t>age_til</t>
+  </si>
+  <si>
+    <t>eur_div</t>
+  </si>
+  <si>
+    <t>dep_acr</t>
+  </si>
+  <si>
+    <t>ono_sen</t>
+  </si>
+  <si>
+    <t>osm_cla</t>
+  </si>
+  <si>
+    <t>lys_cil</t>
+  </si>
+  <si>
+    <t>bot_mul</t>
+  </si>
+  <si>
+    <t>bot_dis</t>
+  </si>
+  <si>
+    <t>dry_cri</t>
+  </si>
+  <si>
+    <t>dry_int</t>
+  </si>
+  <si>
+    <t>dry_mar</t>
+  </si>
+  <si>
+    <t>den_pun</t>
+  </si>
+  <si>
+    <t>osm_cin</t>
+  </si>
+  <si>
+    <t>den_den</t>
+  </si>
+  <si>
+    <t>spi_ann</t>
+  </si>
+  <si>
+    <t>phe_con</t>
+  </si>
+  <si>
+    <t>pol_acr</t>
+  </si>
+  <si>
+    <t>pte_aqu</t>
+  </si>
+  <si>
+    <t>the_nov</t>
+  </si>
+  <si>
+    <t>den_obs</t>
+  </si>
+  <si>
+    <t>dip_com</t>
+  </si>
+  <si>
+    <t>dip_dig</t>
+  </si>
+  <si>
+    <t>lyc_cla</t>
   </si>
 </sst>
 </file>
@@ -933,7 +1002,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,6 +1043,9 @@
       <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="E2" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1022,6 +1094,9 @@
       <c r="D5" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="E5" s="7" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1053,6 +1128,9 @@
       <c r="D7" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="E7" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1169,6 +1247,9 @@
       <c r="D14" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="E14" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -1183,6 +1264,9 @@
       <c r="D15" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="E15" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -1197,8 +1281,11 @@
       <c r="D16" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -1211,8 +1298,11 @@
       <c r="D17" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1225,8 +1315,11 @@
       <c r="D18" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1239,8 +1332,11 @@
       <c r="D19" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1253,8 +1349,11 @@
       <c r="D20" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1267,8 +1366,11 @@
       <c r="D21" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1281,8 +1383,11 @@
       <c r="D22" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -1295,8 +1400,11 @@
       <c r="D23" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
@@ -1309,8 +1417,11 @@
       <c r="D24" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
@@ -1323,8 +1434,11 @@
       <c r="D25" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
@@ -1337,8 +1451,11 @@
       <c r="D26" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
@@ -1351,8 +1468,11 @@
       <c r="D27" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
@@ -1365,8 +1485,11 @@
       <c r="D28" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
@@ -1379,8 +1502,11 @@
       <c r="D29" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
@@ -1393,8 +1519,11 @@
       <c r="D30" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>34</v>
       </c>
@@ -1407,8 +1536,11 @@
       <c r="D31" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
@@ -1421,8 +1553,11 @@
       <c r="D32" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
@@ -1434,6 +1569,9 @@
       </c>
       <c r="D33" s="3" t="s">
         <v>1</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>